<commit_message>
changed fragment duration test. updated results
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CS518\LowLatency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B14C78-48DA-4B13-BB33-0EEAAA62CF17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC25AEA-E297-4D49-85DF-7D742047229A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3885" yWindow="2610" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>keyframe</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Live Latency</t>
+  </si>
+  <si>
+    <t>Buffer Length</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -381,7 +384,7 @@
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +406,11 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -418,7 +424,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
@@ -432,7 +438,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90</v>
       </c>
@@ -446,7 +452,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>120</v>
       </c>
@@ -460,7 +466,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>150</v>
       </c>
@@ -474,7 +480,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>180</v>
       </c>
@@ -488,7 +494,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>120</v>
       </c>
@@ -505,7 +511,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>120</v>
       </c>
@@ -513,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>6.5</v>
+        <v>7.5</v>
       </c>
       <c r="E10">
         <v>6.6000000000000003E-2</v>
@@ -522,7 +528,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>120</v>
       </c>
@@ -530,7 +536,7 @@
         <v>4</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11">
         <v>6.3090000000000002</v>
@@ -545,7 +551,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>120</v>
       </c>
@@ -553,7 +559,7 @@
         <v>4</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>0.2</v>
@@ -562,12 +568,15 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
       <c r="B13">
         <v>4</v>
+      </c>
+      <c r="C13">
+        <v>15</v>
       </c>
       <c r="E13">
         <v>0.5</v>
@@ -576,12 +585,15 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
       <c r="B14">
         <v>4</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -589,13 +601,19 @@
       <c r="F14">
         <v>2000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>120</v>
       </c>
       <c r="B15">
         <v>4</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -603,8 +621,11 @@
       <c r="F15">
         <v>2000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>120</v>
       </c>

</xml_diff>

<commit_message>
modified script to test different settings
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CS518\LowLatency\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC25AEA-E297-4D49-85DF-7D742047229A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B677556E-FF5D-434F-8B08-1483E7B14C64}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3525" yWindow="2310" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -45,10 +45,10 @@
     <t>Segment Size (KB)</t>
   </si>
   <si>
-    <t>Live Latency</t>
-  </si>
-  <si>
     <t>Buffer Length</t>
+  </si>
+  <si>
+    <t>Not Chunked</t>
   </si>
 </sst>
 </file>
@@ -369,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,11 +380,10 @@
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -395,22 +394,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30</v>
       </c>
@@ -420,11 +419,17 @@
       <c r="C2">
         <v>2.5</v>
       </c>
-      <c r="F2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2000</v>
+      </c>
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>60</v>
       </c>
@@ -434,11 +439,17 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="F3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2000</v>
+      </c>
+      <c r="I3">
+        <v>6.5</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>90</v>
       </c>
@@ -448,11 +459,17 @@
       <c r="C4">
         <v>4.2</v>
       </c>
-      <c r="F4">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>2000</v>
+      </c>
+      <c r="I4">
+        <v>5</v>
+      </c>
+      <c r="L4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>120</v>
       </c>
@@ -462,11 +479,17 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="F5">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>2000</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>150</v>
       </c>
@@ -476,11 +499,17 @@
       <c r="C6">
         <v>6</v>
       </c>
-      <c r="F6">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>2000</v>
+      </c>
+      <c r="I6">
+        <v>6.5</v>
+      </c>
+      <c r="L6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>180</v>
       </c>
@@ -490,11 +519,17 @@
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="F7">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>2000</v>
+      </c>
+      <c r="I7">
+        <v>6.5</v>
+      </c>
+      <c r="L7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>120</v>
       </c>
@@ -504,14 +539,17 @@
       <c r="C9">
         <v>6.5</v>
       </c>
+      <c r="D9">
+        <v>3.3000000000000002E-2</v>
+      </c>
       <c r="E9">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F9">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+      <c r="I9">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>120</v>
       </c>
@@ -521,14 +559,14 @@
       <c r="C10">
         <v>7.5</v>
       </c>
+      <c r="D10">
+        <v>6.6000000000000003E-2</v>
+      </c>
       <c r="E10">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F10">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>120</v>
       </c>
@@ -539,19 +577,16 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>6.3090000000000002</v>
+        <v>0.1</v>
       </c>
       <c r="E11">
-        <v>0.1</v>
+        <v>2000</v>
       </c>
       <c r="F11">
-        <v>2000</v>
-      </c>
-      <c r="G11">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>120</v>
       </c>
@@ -561,14 +596,14 @@
       <c r="C12">
         <v>12</v>
       </c>
+      <c r="D12">
+        <v>0.2</v>
+      </c>
       <c r="E12">
-        <v>0.2</v>
-      </c>
-      <c r="F12">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>120</v>
       </c>
@@ -578,14 +613,14 @@
       <c r="C13">
         <v>15</v>
       </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
       <c r="E13">
-        <v>0.5</v>
-      </c>
-      <c r="F13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>120</v>
       </c>
@@ -595,17 +630,17 @@
       <c r="C14">
         <v>20</v>
       </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>2000</v>
-      </c>
-      <c r="H14">
+        <v>2000</v>
+      </c>
+      <c r="G14">
         <v>0.2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>120</v>
       </c>
@@ -615,27 +650,27 @@
       <c r="C15">
         <v>25</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
       <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>2000</v>
-      </c>
-      <c r="H15">
+        <v>2000</v>
+      </c>
+      <c r="G15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>120</v>
       </c>
       <c r="B16">
         <v>4</v>
       </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
       <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
         <v>2000</v>
       </c>
     </row>

</xml_diff>